<commit_message>
ready for day 2
</commit_message>
<xml_diff>
--- a/files/foo.xlsx
+++ b/files/foo.xlsx
@@ -468,60 +468,60 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>0.1274809649855506</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.978857229460504</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.5939427792866853</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.6939023029213166</v>
-      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.7386651917004153</v>
+        <v>0.4002772348174767</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7034213841536741</v>
+        <v>0.5431348647183788</v>
       </c>
       <c r="D4" t="n">
-        <v>0.7465299559420527</v>
+        <v>0.7886513243237703</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3168995376117015</v>
+        <v>0.1983021219847731</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="B5" t="n">
+        <v>0.2946906611286113</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.7509706769625255</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.6277136061112309</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.6820443385204394</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.05214057788492543</v>
+        <v>0.2221659431358408</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5490168806563402</v>
+        <v>0.5873160119473396</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6989399454424667</v>
+        <v>0.2318650345370438</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1777873115857204</v>
+        <v>0.2233401124591544</v>
       </c>
     </row>
     <row r="7">
@@ -529,16 +529,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.7418367923258693</v>
+        <v>0.05231955695830004</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8535530724793429</v>
+        <v>0.9163739752124588</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2399862775497102</v>
+        <v>0.460125088921839</v>
       </c>
       <c r="E7" t="n">
-        <v>0.910084299710058</v>
+        <v>0.3943265412458657</v>
       </c>
     </row>
     <row r="8">
@@ -546,16 +546,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.1536634468188682</v>
+        <v>0.0119699462578432</v>
       </c>
       <c r="C8" t="n">
-        <v>0.06468379652734457</v>
+        <v>0.9681531945047134</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3615500317896642</v>
+        <v>0.3850480984353858</v>
       </c>
       <c r="E8" t="n">
-        <v>0.351468102826467</v>
+        <v>0.7769529032977942</v>
       </c>
     </row>
     <row r="9">
@@ -563,16 +563,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.4410640897737587</v>
+        <v>0.09596340882460686</v>
       </c>
       <c r="C9" t="n">
-        <v>0.3012252948576796</v>
+        <v>0.8594424714340876</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6046755120919328</v>
+        <v>0.09025011991474496</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2581797518749128</v>
+        <v>0.1465547978935255</v>
       </c>
     </row>
     <row r="10">
@@ -580,16 +580,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.05923723549896454</v>
+        <v>0.05480131625056961</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9864420233246822</v>
+        <v>0.7107469028220068</v>
       </c>
       <c r="D10" t="n">
-        <v>0.963252434172845</v>
+        <v>0.7390505873732331</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1044594993945814</v>
+        <v>0.2859386108804015</v>
       </c>
     </row>
     <row r="11">
@@ -597,16 +597,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.1046960025911664</v>
+        <v>0.06422856648110331</v>
       </c>
       <c r="C11" t="n">
-        <v>0.7357804224092772</v>
+        <v>0.7679801630257539</v>
       </c>
       <c r="D11" t="n">
-        <v>0.8856657318251637</v>
+        <v>0.6079700923505065</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9669039873975606</v>
+        <v>0.325544513299205</v>
       </c>
     </row>
     <row r="12">
@@ -614,42 +614,50 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.3760223318759597</v>
+        <v>0.07365581671163701</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1330967906023314</v>
+        <v>0.8252134232295009</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3067945875437567</v>
+        <v>0.4768895973277797</v>
       </c>
       <c r="E12" t="n">
-        <v>0.6032407401018482</v>
+        <v>0.3651504157180084</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
+      <c r="B13" t="n">
+        <v>0.08308306694217071</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.8824466834332478</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.345809102305053</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.4047563181368118</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.9387786089830513</v>
+        <v>0.09251031717270441</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6625049321472801</v>
+        <v>0.9396799436369949</v>
       </c>
       <c r="D14" t="n">
-        <v>0.417972944777619</v>
+        <v>0.2147286072823262</v>
       </c>
       <c r="E14" t="n">
-        <v>0.8079033458994578</v>
+        <v>0.4443622205556153</v>
       </c>
     </row>
     <row r="15">
@@ -657,16 +665,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.7822088902196297</v>
+        <v>0.135165339552934</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6534675441408242</v>
+        <v>0.5607200016458863</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2351165679255481</v>
+        <v>0.4009313365275903</v>
       </c>
       <c r="E15" t="n">
-        <v>0.7051537432995025</v>
+        <v>0.5796378777642874</v>
       </c>
     </row>
     <row r="16">
@@ -674,16 +682,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.7059646443073352</v>
+        <v>0.6907932158480315</v>
       </c>
       <c r="C16" t="n">
-        <v>0.7617030089110396</v>
+        <v>0.7573630362045051</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0008905815536571771</v>
+        <v>0.7557610640945464</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9644741308267746</v>
+        <v>0.197494817332417</v>
       </c>
     </row>
     <row r="17">
@@ -691,16 +699,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.02478257249388449</v>
+        <v>0.5897160456816568</v>
       </c>
       <c r="C17" t="n">
-        <v>0.9220696796903189</v>
+        <v>0.8325245464970247</v>
       </c>
       <c r="D17" t="n">
-        <v>0.8749085814918759</v>
+        <v>0.5422165271291751</v>
       </c>
       <c r="E17" t="n">
-        <v>0.162928826596183</v>
+        <v>0.3455607618129297</v>
       </c>
     </row>
     <row r="18">
@@ -708,16 +716,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.6995113608011553</v>
+        <v>0.488638875515282</v>
       </c>
       <c r="C18" t="n">
-        <v>0.9453523792274418</v>
+        <v>0.9076860567895444</v>
       </c>
       <c r="D18" t="n">
-        <v>0.9888141009929617</v>
+        <v>0.3286719901638039</v>
       </c>
       <c r="E18" t="n">
-        <v>0.01431000900014179</v>
+        <v>0.4936267062934425</v>
       </c>
     </row>
     <row r="19">
@@ -725,16 +733,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.2430388951178257</v>
+        <v>0.3875617053489072</v>
       </c>
       <c r="C19" t="n">
-        <v>0.8452645428746706</v>
+        <v>0.982847567082064</v>
       </c>
       <c r="D19" t="n">
-        <v>0.636678753118025</v>
+        <v>0.1151274531984326</v>
       </c>
       <c r="E19" t="n">
-        <v>0.6181269827254275</v>
+        <v>0.6416926507739552</v>
       </c>
     </row>
     <row r="20">
@@ -742,16 +750,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.492308451165625</v>
+        <v>0.8862605938668301</v>
       </c>
       <c r="C20" t="n">
-        <v>0.9707168264323968</v>
+        <v>0.7270351856955494</v>
       </c>
       <c r="D20" t="n">
-        <v>0.83767166996787</v>
+        <v>0.6499926272132465</v>
       </c>
       <c r="E20" t="n">
-        <v>0.3335562180829775</v>
+        <v>0.3452828256819239</v>
       </c>
     </row>
     <row r="21">
@@ -759,16 +767,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.2988061663863758</v>
+        <v>0.9475179683522807</v>
       </c>
       <c r="C21" t="n">
-        <v>0.120042594501893</v>
+        <v>0.6574841711212315</v>
       </c>
       <c r="D21" t="n">
-        <v>0.1256208086542566</v>
+        <v>0.1477722063434623</v>
       </c>
       <c r="E21" t="n">
-        <v>0.6820916888362165</v>
+        <v>0.2268406064517345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>